<commit_message>
completed builder and factory for domain
Signed-off-by: aditya109 <adikid1996@gmail.com>
</commit_message>
<xml_diff>
--- a/1.3/server/assets/cpnc/cpnc.xlsx
+++ b/1.3/server/assets/cpnc/cpnc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kidad\Desktop\cpnc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\bank-reconcilation-statement-validator\1.3\server\assets\cpnc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="1">
   <si>
     <t>CASH</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -368,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1881"/>
+  <dimension ref="A1:C1880"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A1873" workbookViewId="0">
+      <selection activeCell="D1892" sqref="D1892"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21061,15 +21058,6 @@
         <v>5632474</v>
       </c>
     </row>
-    <row r="1881" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1881" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1881" s="3">
-        <f>SUM(C1:C1880)</f>
-        <v>119096489.89</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>